<commit_message>
4.1 - template change and added build date
</commit_message>
<xml_diff>
--- a/Runtime/Templates/Template.xlsx
+++ b/Runtime/Templates/Template.xlsx
@@ -556,173 +556,173 @@
   </cellStyleXfs>
   <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1114,7 +1114,7 @@
   <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:E9"/>
+      <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1127,1099 +1127,1131 @@
     <col min="6" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="18"/>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="str">
-        <f ca="1" xml:space="preserve"> "CREATED ON: " &amp; TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>CREATED ON: 06/09/2017</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="24"/>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="str">
+        <f xml:space="preserve"> "CREATED ON: "</f>
+        <v xml:space="preserve">CREATED ON: </v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="27"/>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="20"/>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="20"/>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="29"/>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="55"/>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="31"/>
-    </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
-    </row>
-    <row r="13" spans="1:5" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="48"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="50"/>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="47" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="47" t="s">
+      <c r="A21" s="26"/>
+      <c r="B21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="47" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="47" t="s">
+      <c r="A27" s="28"/>
+      <c r="B27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="47" t="s">
+      <c r="A28" s="28"/>
+      <c r="B28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="47" t="s">
+      <c r="A30" s="28"/>
+      <c r="B30" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="47" t="s">
+      <c r="A31" s="28"/>
+      <c r="B31" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
-      <c r="B33" s="47" t="s">
+      <c r="A33" s="28"/>
+      <c r="B33" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
-      <c r="B34" s="47" t="s">
+      <c r="A34" s="28"/>
+      <c r="B34" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
-      <c r="B36" s="47" t="s">
+      <c r="A36" s="28"/>
+      <c r="B36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="47" t="s">
+      <c r="A37" s="28"/>
+      <c r="B37" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="37"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="39"/>
-      <c r="B40" s="47" t="s">
+      <c r="A40" s="25"/>
+      <c r="B40" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="40"/>
-      <c r="B41" s="47" t="s">
+      <c r="A41" s="26"/>
+      <c r="B41" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="58" t="s">
+      <c r="B42" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="39"/>
-      <c r="B43" s="47" t="s">
+      <c r="A43" s="25"/>
+      <c r="B43" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
-      <c r="B44" s="47" t="s">
+      <c r="A44" s="26"/>
+      <c r="B44" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="39"/>
-      <c r="B46" s="47" t="s">
+      <c r="A46" s="25"/>
+      <c r="B46" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="40"/>
-      <c r="B47" s="47" t="s">
+      <c r="A47" s="26"/>
+      <c r="B47" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="39"/>
-      <c r="B49" s="47" t="s">
+      <c r="A49" s="25"/>
+      <c r="B49" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="40"/>
-      <c r="B50" s="47" t="s">
+      <c r="A50" s="26"/>
+      <c r="B50" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B51" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="39"/>
-      <c r="B52" s="47" t="s">
+      <c r="A52" s="25"/>
+      <c r="B52" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="40"/>
-      <c r="B53" s="47" t="s">
+      <c r="A53" s="26"/>
+      <c r="B53" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
+      <c r="A54" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="58" t="s">
+      <c r="B54" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="47"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="39"/>
-      <c r="B55" s="47" t="s">
+      <c r="A55" s="25"/>
+      <c r="B55" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="40"/>
-      <c r="B56" s="47" t="s">
+      <c r="A56" s="26"/>
+      <c r="B56" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="s">
+      <c r="A57" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="58" t="s">
+      <c r="B57" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="39"/>
-      <c r="B58" s="47" t="s">
+      <c r="A58" s="25"/>
+      <c r="B58" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="40"/>
-      <c r="B59" s="47" t="s">
+      <c r="A59" s="26"/>
+      <c r="B59" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
+      <c r="A60" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="58" t="s">
+      <c r="B60" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="39"/>
-      <c r="B61" s="47" t="s">
+      <c r="A61" s="25"/>
+      <c r="B61" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="40"/>
-      <c r="B62" s="47" t="s">
+      <c r="A62" s="26"/>
+      <c r="B62" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="38" t="s">
+      <c r="A63" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B63" s="58" t="s">
+      <c r="B63" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="39"/>
-      <c r="B64" s="47" t="s">
+      <c r="A64" s="25"/>
+      <c r="B64" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="40"/>
-      <c r="B65" s="47" t="s">
+      <c r="A65" s="26"/>
+      <c r="B65" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="38" t="s">
+      <c r="A66" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B66" s="58" t="s">
+      <c r="B66" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="39"/>
-      <c r="B67" s="47" t="s">
+      <c r="A67" s="25"/>
+      <c r="B67" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C67" s="47"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="47"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="40"/>
-      <c r="B68" s="47" t="s">
+      <c r="A68" s="26"/>
+      <c r="B68" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="38" t="s">
+      <c r="A69" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="39"/>
-      <c r="B70" s="47" t="s">
+      <c r="A70" s="25"/>
+      <c r="B70" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C70" s="47"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="40"/>
-      <c r="B71" s="47" t="s">
+      <c r="A71" s="26"/>
+      <c r="B71" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="47"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="38" t="s">
+      <c r="A72" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B72" s="58" t="s">
+      <c r="B72" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="39"/>
-      <c r="B73" s="47" t="s">
+      <c r="A73" s="25"/>
+      <c r="B73" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
-      <c r="E73" s="47"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="40"/>
-      <c r="B74" s="47" t="s">
+      <c r="A74" s="26"/>
+      <c r="B74" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="38" t="s">
+      <c r="A75" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B75" s="58" t="s">
+      <c r="B75" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="39"/>
-      <c r="B76" s="47" t="s">
+      <c r="A76" s="25"/>
+      <c r="B76" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C76" s="47"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="40"/>
-      <c r="B77" s="47" t="s">
+      <c r="A77" s="26"/>
+      <c r="B77" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C77" s="47"/>
-      <c r="D77" s="47"/>
-      <c r="E77" s="47"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="37" t="s">
+      <c r="A78" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="27"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="58" t="s">
+      <c r="B79" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C79" s="47"/>
-      <c r="D79" s="47"/>
-      <c r="E79" s="47"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="41"/>
-      <c r="B80" s="47" t="s">
+      <c r="A80" s="28"/>
+      <c r="B80" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C80" s="47"/>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="41"/>
-      <c r="B81" s="47" t="s">
+      <c r="A81" s="28"/>
+      <c r="B81" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C81" s="47"/>
-      <c r="D81" s="47"/>
-      <c r="E81" s="47"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="41" t="s">
+      <c r="A82" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B82" s="58" t="s">
+      <c r="B82" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C82" s="47"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="41"/>
-      <c r="B83" s="47" t="s">
+      <c r="A83" s="28"/>
+      <c r="B83" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C83" s="47"/>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="38"/>
-      <c r="B84" s="47" t="s">
+      <c r="A84" s="24"/>
+      <c r="B84" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C84" s="47"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="42"/>
-      <c r="B85" s="42"/>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="42"/>
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
     </row>
     <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="43" t="s">
+      <c r="A86" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B86" s="43"/>
-      <c r="C86" s="43"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="43"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="30"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="44" t="s">
+      <c r="A87" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B87" s="47" t="s">
+      <c r="B87" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C87" s="47"/>
-      <c r="D87" s="47"/>
-      <c r="E87" s="47"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="44"/>
-      <c r="B88" s="47" t="s">
+      <c r="A88" s="16"/>
+      <c r="B88" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C88" s="47"/>
-      <c r="D88" s="47"/>
-      <c r="E88" s="47"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
     </row>
     <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="45" t="s">
+      <c r="A89" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B89" s="47" t="s">
+      <c r="B89" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C89" s="47"/>
-      <c r="D89" s="47"/>
-      <c r="E89" s="47"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="46"/>
-      <c r="B90" s="46"/>
-      <c r="C90" s="46"/>
-      <c r="D90" s="46"/>
-      <c r="E90" s="46"/>
+      <c r="A90" s="17"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
     </row>
     <row r="91" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="48" t="s">
+      <c r="A91" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="50"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="20"/>
     </row>
     <row r="92" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="51" t="s">
+      <c r="A92" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B92" s="47" t="s">
+      <c r="B92" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C92" s="47"/>
-      <c r="D92" s="47"/>
-      <c r="E92" s="47"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
     </row>
     <row r="93" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="51" t="s">
+      <c r="A93" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B93" s="47" t="s">
+      <c r="B93" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C93" s="47"/>
-      <c r="D93" s="47"/>
-      <c r="E93" s="47"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
     </row>
     <row r="94" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="51" t="s">
+      <c r="A94" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B94" s="47" t="s">
+      <c r="B94" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C94" s="47"/>
-      <c r="D94" s="47"/>
-      <c r="E94" s="47"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="51" t="s">
+      <c r="A95" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B95" s="47" t="s">
+      <c r="B95" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C95" s="47"/>
-      <c r="D95" s="47"/>
-      <c r="E95" s="47"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
     </row>
     <row r="96" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="51" t="s">
+      <c r="A96" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B96" s="47" t="s">
+      <c r="B96" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C96" s="47"/>
-      <c r="D96" s="47"/>
-      <c r="E96" s="47"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
     </row>
     <row r="97" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="51" t="s">
+      <c r="A97" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B97" s="47" t="s">
+      <c r="B97" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C97" s="47"/>
-      <c r="D97" s="47"/>
-      <c r="E97" s="47"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
     </row>
     <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="51" t="s">
+      <c r="A98" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B98" s="47" t="s">
+      <c r="B98" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C98" s="47"/>
-      <c r="D98" s="47"/>
-      <c r="E98" s="47"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="51" t="s">
+      <c r="A99" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B99" s="47" t="s">
+      <c r="B99" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C99" s="47"/>
-      <c r="D99" s="47"/>
-      <c r="E99" s="47"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
     </row>
     <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="51" t="s">
+      <c r="A100" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B100" s="47" t="s">
+      <c r="B100" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C100" s="47"/>
-      <c r="D100" s="47"/>
-      <c r="E100" s="47"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
     </row>
     <row r="101" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="51" t="s">
+      <c r="A101" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B101" s="47" t="s">
+      <c r="B101" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C101" s="47"/>
-      <c r="D101" s="47"/>
-      <c r="E101" s="47"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
     </row>
     <row r="102" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="51" t="s">
+      <c r="A102" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B102" s="47" t="s">
+      <c r="B102" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C102" s="47"/>
-      <c r="D102" s="47"/>
-      <c r="E102" s="47"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="52"/>
-      <c r="B103" s="52"/>
-      <c r="C103" s="52"/>
-      <c r="D103" s="52"/>
-      <c r="E103" s="52"/>
+      <c r="A103" s="21"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
     </row>
     <row r="104" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="53" t="s">
+      <c r="A104" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B104" s="53"/>
-      <c r="C104" s="53"/>
-      <c r="D104" s="53"/>
-      <c r="E104" s="53"/>
+      <c r="B104" s="22"/>
+      <c r="C104" s="22"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="22"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="54" t="s">
+      <c r="A105" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B105" s="47" t="s">
+      <c r="B105" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C105" s="47"/>
-      <c r="D105" s="47"/>
-      <c r="E105" s="47"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="54"/>
-      <c r="B106" s="47" t="s">
+      <c r="A106" s="23"/>
+      <c r="B106" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C106" s="47"/>
-      <c r="D106" s="47"/>
-      <c r="E106" s="47"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="54"/>
-      <c r="B107" s="47" t="s">
+      <c r="A107" s="23"/>
+      <c r="B107" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="47"/>
-      <c r="D107" s="47"/>
-      <c r="E107" s="47"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="54"/>
-      <c r="B108" s="47" t="s">
+      <c r="A108" s="23"/>
+      <c r="B108" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C108" s="47"/>
-      <c r="D108" s="47"/>
-      <c r="E108" s="47"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="54"/>
-      <c r="B109" s="47" t="s">
+      <c r="A109" s="23"/>
+      <c r="B109" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C109" s="47"/>
-      <c r="D109" s="47"/>
-      <c r="E109" s="47"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="54"/>
-      <c r="B110" s="47" t="s">
+      <c r="A110" s="23"/>
+      <c r="B110" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C110" s="47"/>
-      <c r="D110" s="47"/>
-      <c r="E110" s="47"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="54"/>
-      <c r="B111" s="47" t="s">
+      <c r="A111" s="23"/>
+      <c r="B111" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C111" s="47"/>
-      <c r="D111" s="47"/>
-      <c r="E111" s="47"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
     </row>
     <row r="112" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="55" t="s">
+      <c r="A112" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B112" s="47" t="s">
+      <c r="B112" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C112" s="47"/>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
     </row>
     <row r="113" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="56" t="s">
+      <c r="A113" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B113" s="47" t="s">
+      <c r="B113" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C113" s="47"/>
-      <c r="D113" s="47"/>
-      <c r="E113" s="47"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="57"/>
-      <c r="B114" s="57"/>
-      <c r="C114" s="57"/>
-      <c r="D114" s="57"/>
-      <c r="E114" s="57"/>
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
     <mergeCell ref="A114:E114"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A87:A88"/>
@@ -2236,38 +2268,6 @@
     <mergeCell ref="A86:E86"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added error checking for empty input
</commit_message>
<xml_diff>
--- a/Runtime/Templates/Template.xlsx
+++ b/Runtime/Templates/Template.xlsx
@@ -373,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -411,34 +411,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -554,39 +532,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -595,133 +612,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1114,7 +1080,7 @@
   <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E5"/>
+      <selection activeCell="A9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1128,101 +1094,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="str">
-        <f xml:space="preserve"> "CREATED ON: "</f>
-        <v xml:space="preserve">CREATED ON: </v>
-      </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="44"/>
+      <c r="A4" s="29" t="str">
+        <f ca="1" xml:space="preserve"> "CREATED ON " &amp; TEXT(TODAY(),"mm/dd/yyyy") &amp; " FOR BUSINESS DATE:"</f>
+        <v>CREATED ON 07/06/2017 FOR BUSINESS DATE:</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58"/>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1242,25 +1208,25 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -1271,7 +1237,7 @@
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="7" t="s">
         <v>49</v>
       </c>
@@ -1280,7 +1246,7 @@
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="7" t="s">
         <v>50</v>
       </c>
@@ -1289,7 +1255,7 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -1300,7 +1266,7 @@
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="7" t="s">
         <v>49</v>
       </c>
@@ -1309,7 +1275,7 @@
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="7" t="s">
         <v>50</v>
       </c>
@@ -1318,7 +1284,7 @@
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -1329,7 +1295,7 @@
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="7" t="s">
         <v>49</v>
       </c>
@@ -1338,7 +1304,7 @@
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="7" t="s">
         <v>50</v>
       </c>
@@ -1347,16 +1313,16 @@
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -1367,7 +1333,7 @@
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="7" t="s">
         <v>49</v>
       </c>
@@ -1376,7 +1342,7 @@
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="7" t="s">
         <v>50</v>
       </c>
@@ -1385,7 +1351,7 @@
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -1396,7 +1362,7 @@
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="7" t="s">
         <v>49</v>
       </c>
@@ -1405,7 +1371,7 @@
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="7" t="s">
         <v>50</v>
       </c>
@@ -1414,7 +1380,7 @@
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="11" t="s">
@@ -1425,7 +1391,7 @@
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="7" t="s">
         <v>49</v>
       </c>
@@ -1434,7 +1400,7 @@
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="7" t="s">
         <v>50</v>
       </c>
@@ -1443,7 +1409,7 @@
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="42" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -1454,7 +1420,7 @@
       <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="7" t="s">
         <v>49</v>
       </c>
@@ -1463,7 +1429,7 @@
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="7" t="s">
         <v>50</v>
       </c>
@@ -1472,16 +1438,16 @@
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="37"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="23" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="11" t="s">
@@ -1492,7 +1458,7 @@
       <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="7" t="s">
         <v>49</v>
       </c>
@@ -1501,7 +1467,7 @@
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="7" t="s">
         <v>50</v>
       </c>
@@ -1510,7 +1476,7 @@
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="11" t="s">
@@ -1521,7 +1487,7 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="7" t="s">
         <v>49</v>
       </c>
@@ -1530,7 +1496,7 @@
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="7" t="s">
         <v>50</v>
       </c>
@@ -1539,7 +1505,7 @@
       <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B45" s="11" t="s">
@@ -1550,7 +1516,7 @@
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="7" t="s">
         <v>49</v>
       </c>
@@ -1559,7 +1525,7 @@
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="7" t="s">
         <v>50</v>
       </c>
@@ -1568,7 +1534,7 @@
       <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="11" t="s">
@@ -1579,7 +1545,7 @@
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="7" t="s">
         <v>49</v>
       </c>
@@ -1588,7 +1554,7 @@
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="7" t="s">
         <v>50</v>
       </c>
@@ -1597,7 +1563,7 @@
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="23" t="s">
         <v>24</v>
       </c>
       <c r="B51" s="11" t="s">
@@ -1608,7 +1574,7 @@
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="7" t="s">
         <v>49</v>
       </c>
@@ -1617,7 +1583,7 @@
       <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="7" t="s">
         <v>50</v>
       </c>
@@ -1626,7 +1592,7 @@
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
+      <c r="A54" s="23" t="s">
         <v>25</v>
       </c>
       <c r="B54" s="11" t="s">
@@ -1637,7 +1603,7 @@
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="7" t="s">
         <v>49</v>
       </c>
@@ -1646,7 +1612,7 @@
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+      <c r="A56" s="25"/>
       <c r="B56" s="7" t="s">
         <v>50</v>
       </c>
@@ -1655,7 +1621,7 @@
       <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B57" s="11" t="s">
@@ -1666,7 +1632,7 @@
       <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="7" t="s">
         <v>49</v>
       </c>
@@ -1675,7 +1641,7 @@
       <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="7" t="s">
         <v>50</v>
       </c>
@@ -1684,7 +1650,7 @@
       <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B60" s="11" t="s">
@@ -1695,7 +1661,7 @@
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="7" t="s">
         <v>49</v>
       </c>
@@ -1704,7 +1670,7 @@
       <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="7" t="s">
         <v>50</v>
       </c>
@@ -1713,7 +1679,7 @@
       <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="23" t="s">
         <v>28</v>
       </c>
       <c r="B63" s="11" t="s">
@@ -1724,7 +1690,7 @@
       <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="7" t="s">
         <v>49</v>
       </c>
@@ -1733,7 +1699,7 @@
       <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="26"/>
+      <c r="A65" s="25"/>
       <c r="B65" s="7" t="s">
         <v>50</v>
       </c>
@@ -1742,7 +1708,7 @@
       <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B66" s="11" t="s">
@@ -1753,7 +1719,7 @@
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="25"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="7" t="s">
         <v>49</v>
       </c>
@@ -1762,7 +1728,7 @@
       <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="7" t="s">
         <v>50</v>
       </c>
@@ -1771,7 +1737,7 @@
       <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="24" t="s">
+      <c r="A69" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B69" s="11" t="s">
@@ -1782,7 +1748,7 @@
       <c r="E69" s="7"/>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="7" t="s">
         <v>49</v>
       </c>
@@ -1791,7 +1757,7 @@
       <c r="E70" s="7"/>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="7" t="s">
         <v>50</v>
       </c>
@@ -1800,7 +1766,7 @@
       <c r="E71" s="7"/>
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="24" t="s">
+      <c r="A72" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B72" s="11" t="s">
@@ -1811,7 +1777,7 @@
       <c r="E72" s="7"/>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="25"/>
+      <c r="A73" s="24"/>
       <c r="B73" s="7" t="s">
         <v>49</v>
       </c>
@@ -1820,7 +1786,7 @@
       <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="7" t="s">
         <v>50</v>
       </c>
@@ -1829,7 +1795,7 @@
       <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
+      <c r="A75" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B75" s="11" t="s">
@@ -1840,7 +1806,7 @@
       <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="7" t="s">
         <v>49</v>
       </c>
@@ -1849,7 +1815,7 @@
       <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="26"/>
+      <c r="A77" s="25"/>
       <c r="B77" s="7" t="s">
         <v>50</v>
       </c>
@@ -1858,16 +1824,16 @@
       <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="27" t="s">
+      <c r="A78" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
+      <c r="B78" s="52"/>
+      <c r="C78" s="52"/>
+      <c r="D78" s="52"/>
+      <c r="E78" s="52"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="s">
+      <c r="A79" s="42" t="s">
         <v>35</v>
       </c>
       <c r="B79" s="11" t="s">
@@ -1878,7 +1844,7 @@
       <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="28"/>
+      <c r="A80" s="42"/>
       <c r="B80" s="7" t="s">
         <v>49</v>
       </c>
@@ -1887,7 +1853,7 @@
       <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="28"/>
+      <c r="A81" s="42"/>
       <c r="B81" s="7" t="s">
         <v>50</v>
       </c>
@@ -1896,7 +1862,7 @@
       <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
+      <c r="A82" s="42" t="s">
         <v>36</v>
       </c>
       <c r="B82" s="11" t="s">
@@ -1907,7 +1873,7 @@
       <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="28"/>
+      <c r="A83" s="42"/>
       <c r="B83" s="7" t="s">
         <v>49</v>
       </c>
@@ -1916,7 +1882,7 @@
       <c r="E83" s="7"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="24"/>
+      <c r="A84" s="23"/>
       <c r="B84" s="7" t="s">
         <v>50</v>
       </c>
@@ -1925,23 +1891,23 @@
       <c r="E84" s="7"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="29"/>
+      <c r="A85" s="53"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
+      <c r="E85" s="53"/>
     </row>
     <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="30" t="s">
+      <c r="A86" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B86" s="30"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="30"/>
+      <c r="B86" s="54"/>
+      <c r="C86" s="54"/>
+      <c r="D86" s="54"/>
+      <c r="E86" s="54"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
+      <c r="A87" s="44" t="s">
         <v>38</v>
       </c>
       <c r="B87" s="7" t="s">
@@ -1952,7 +1918,7 @@
       <c r="E87" s="7"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="16"/>
+      <c r="A88" s="44"/>
       <c r="B88" s="7" t="s">
         <v>70</v>
       </c>
@@ -1972,20 +1938,20 @@
       <c r="E89" s="7"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
+      <c r="A90" s="45"/>
+      <c r="B90" s="45"/>
+      <c r="C90" s="45"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="45"/>
     </row>
     <row r="91" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="18" t="s">
+      <c r="A91" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B91" s="19"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
-      <c r="E91" s="20"/>
+      <c r="B91" s="47"/>
+      <c r="C91" s="47"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="48"/>
     </row>
     <row r="92" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
@@ -2109,23 +2075,23 @@
       <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="21"/>
-      <c r="B103" s="21"/>
-      <c r="C103" s="21"/>
-      <c r="D103" s="21"/>
-      <c r="E103" s="21"/>
+      <c r="A103" s="49"/>
+      <c r="B103" s="49"/>
+      <c r="C103" s="49"/>
+      <c r="D103" s="49"/>
+      <c r="E103" s="49"/>
     </row>
     <row r="104" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="22" t="s">
+      <c r="A104" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B104" s="22"/>
-      <c r="C104" s="22"/>
-      <c r="D104" s="22"/>
-      <c r="E104" s="22"/>
+      <c r="B104" s="50"/>
+      <c r="C104" s="50"/>
+      <c r="D104" s="50"/>
+      <c r="E104" s="50"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="23" t="s">
+      <c r="A105" s="51" t="s">
         <v>46</v>
       </c>
       <c r="B105" s="7" t="s">
@@ -2136,7 +2102,7 @@
       <c r="E105" s="7"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="23"/>
+      <c r="A106" s="51"/>
       <c r="B106" s="7" t="s">
         <v>73</v>
       </c>
@@ -2145,7 +2111,7 @@
       <c r="E106" s="7"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="23"/>
+      <c r="A107" s="51"/>
       <c r="B107" s="7" t="s">
         <v>74</v>
       </c>
@@ -2154,7 +2120,7 @@
       <c r="E107" s="7"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="23"/>
+      <c r="A108" s="51"/>
       <c r="B108" s="7" t="s">
         <v>75</v>
       </c>
@@ -2163,7 +2129,7 @@
       <c r="E108" s="7"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="23"/>
+      <c r="A109" s="51"/>
       <c r="B109" s="7" t="s">
         <v>76</v>
       </c>
@@ -2172,7 +2138,7 @@
       <c r="E109" s="7"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="23"/>
+      <c r="A110" s="51"/>
       <c r="B110" s="7" t="s">
         <v>77</v>
       </c>
@@ -2181,7 +2147,7 @@
       <c r="E110" s="7"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="23"/>
+      <c r="A111" s="51"/>
       <c r="B111" s="7" t="s">
         <v>78</v>
       </c>
@@ -2212,48 +2178,18 @@
       <c r="E113" s="7"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="12"/>
-      <c r="B114" s="12"/>
-      <c r="C114" s="12"/>
-      <c r="D114" s="12"/>
-      <c r="E114" s="12"/>
+      <c r="A114" s="43"/>
+      <c r="B114" s="43"/>
+      <c r="C114" s="43"/>
+      <c r="D114" s="43"/>
+      <c r="E114" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A114:E114"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A114:E114"/>
-    <mergeCell ref="A6:E6"/>
     <mergeCell ref="A87:A88"/>
     <mergeCell ref="A90:E90"/>
     <mergeCell ref="A91:E91"/>
@@ -2268,6 +2204,36 @@
     <mergeCell ref="A86:E86"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>